<commit_message>
Updated TC5 for multiplicative
</commit_message>
<xml_diff>
--- a/Test Case - 3/TC3_Results_1.xlsx
+++ b/Test Case - 3/TC3_Results_1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="outfile" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1007,20 +1007,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1066,7 +1066,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1094,36 +1094,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1406,92 +1376,92 @@
   <dimension ref="A1:S116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="6" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="4" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="6" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2708,7 +2678,7 @@
       <c r="L24">
         <v>79</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24" s="3">
         <v>0</v>
       </c>
       <c r="N24">
@@ -2726,7 +2696,7 @@
       <c r="R24">
         <v>35.152000000000001</v>
       </c>
-      <c r="S24" s="8">
+      <c r="S24" s="5">
         <f>0.9*((R24-D24)^0.51)*((SQRT((P24-B24)^2+(Q24-C24)^2)^(-0.35)))</f>
         <v>2.8488243388147674</v>
       </c>
@@ -3290,8 +3260,8 @@
       <c r="R34">
         <v>35.152000000000001</v>
       </c>
-      <c r="S34" s="7">
-        <f t="shared" ref="S26:S34" si="0">0.9*((R34-D34)^0.51)*((SQRT((P34-B34)^2+(Q34-C34)^2)^(-0.35)))</f>
+      <c r="S34" s="4">
+        <f t="shared" ref="S34" si="0">0.9*((R34-D34)^0.51)*((SQRT((P34-B34)^2+(Q34-C34)^2)^(-0.35)))</f>
         <v>1.486934389517961</v>
       </c>
     </row>
@@ -3332,7 +3302,7 @@
       <c r="L35">
         <v>46</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M35" s="3">
         <v>0</v>
       </c>
       <c r="N35">
@@ -3341,7 +3311,7 @@
       <c r="O35" t="b">
         <v>0</v>
       </c>
-      <c r="S35" s="8"/>
+      <c r="S35" s="5"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -3790,7 +3760,7 @@
       <c r="R43">
         <v>35.152000000000001</v>
       </c>
-      <c r="S43" s="7">
+      <c r="S43" s="4">
         <f t="shared" ref="S43:S44" si="1">0.9*((R43-D43)^0.51)*((SQRT((P43-B43)^2+(Q43-C43)^2)^(-0.35)))</f>
         <v>1.1644085258098895</v>
       </c>
@@ -3850,7 +3820,7 @@
       <c r="R44">
         <v>35.152000000000001</v>
       </c>
-      <c r="S44" s="7">
+      <c r="S44" s="4">
         <f t="shared" si="1"/>
         <v>1.4896628100405325</v>
       </c>
@@ -6262,7 +6232,7 @@
       <c r="R87">
         <v>37.652000000000001</v>
       </c>
-      <c r="S87" s="8">
+      <c r="S87" s="5">
         <f t="shared" ref="S87" si="2">0.9*((R87-D87)^0.51)*((SQRT((P87-B87)^2+(Q87-C87)^2)^(-0.35)))</f>
         <v>0.93101418279599779</v>
       </c>
@@ -7605,6 +7575,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="K1:K2"/>
@@ -7613,12 +7589,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="O3:O116">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">

</xml_diff>